<commit_message>
Started working on Version 2 of the PCB. Added KiCAD component library submodule.
</commit_message>
<xml_diff>
--- a/KiCad/Ver2/Outputs/BOM_Planning.xlsx
+++ b/KiCad/Ver2/Outputs/BOM_Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="30876" windowHeight="20064"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="16200" windowHeight="11076"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -107,19 +107,82 @@
     <t>C5947</t>
   </si>
   <si>
-    <t>SOIC-17</t>
-  </si>
-  <si>
     <t>74HC595</t>
   </si>
   <si>
-    <t>74HC596</t>
-  </si>
-  <si>
     <t>74HC595,118</t>
   </si>
   <si>
     <t>74HC595,119</t>
+  </si>
+  <si>
+    <t>Octal Buffer</t>
+  </si>
+  <si>
+    <t>74HC244</t>
+  </si>
+  <si>
+    <t>TSSOP-20</t>
+  </si>
+  <si>
+    <t>C5623</t>
+  </si>
+  <si>
+    <t>74HC244PW,118</t>
+  </si>
+  <si>
+    <t>Digital Switch IC</t>
+  </si>
+  <si>
+    <t>74LVC1G3157</t>
+  </si>
+  <si>
+    <t>SC-88</t>
+  </si>
+  <si>
+    <t>74LVC1G3157GW,125</t>
+  </si>
+  <si>
+    <t>C426706</t>
+  </si>
+  <si>
+    <t>Rectification Diodes</t>
+  </si>
+  <si>
+    <t>C108803</t>
+  </si>
+  <si>
+    <t>1N4007W</t>
+  </si>
+  <si>
+    <t>1N4007</t>
+  </si>
+  <si>
+    <t>SOD-123F</t>
+  </si>
+  <si>
+    <t>High Voltage Drive Switch</t>
+  </si>
+  <si>
+    <t>C36220</t>
+  </si>
+  <si>
+    <t>AOD409</t>
+  </si>
+  <si>
+    <t>TO-252-2(DPAK)</t>
+  </si>
+  <si>
+    <t>C59981</t>
+  </si>
+  <si>
+    <t>Board To Board Connector (Male)</t>
+  </si>
+  <si>
+    <t>C124397</t>
+  </si>
+  <si>
+    <t>Board To Board Connector (Female)</t>
   </si>
 </sst>
 </file>
@@ -173,10 +236,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,39 +528,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -506,7 +574,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
@@ -523,7 +591,7 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
@@ -540,7 +608,7 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" t="s">
@@ -560,7 +628,7 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E5" t="s">
@@ -572,16 +640,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -589,16 +657,100 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -609,8 +761,14 @@
     <hyperlink ref="D5" r:id="rId4" display="https://lcsc.com/product-detail/74-Series_Nexperia_74HC165D-653_74HC165D-653_C5613.html/?href=jlc-SMT"/>
     <hyperlink ref="D6" r:id="rId5" display="https://lcsc.com/product-detail/74-Series_Nexperia-74HC595D-118_C5947.html/?href=jlc-SMT"/>
     <hyperlink ref="D7" r:id="rId6" display="https://lcsc.com/product-detail/74-Series_Nexperia-74HC595D-118_C5947.html/?href=jlc-SMT"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>